<commit_message>
Tried to merge files. Did not work. Error in that it is estimating that the PT depth is more than the actual depth. Need to fix. Also, low pt depths need flow estimate for small intervals.
</commit_message>
<xml_diff>
--- a/Data/Stormwaterexport_cfs.xlsx
+++ b/Data/Stormwaterexport_cfs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="262" documentId="11_4AB480A97D773D78B6F332151CC35944F734729B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D95A272B-2D05-42C1-8515-97D58A5D2076}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51E3D54-1F92-459B-BE7D-9991FAE2605A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16350" yWindow="465" windowWidth="31320" windowHeight="20535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -84,17 +82,23 @@
     <t>water level was too high to get a true measurement, some measurements are estimated.</t>
   </si>
   <si>
-    <t>10:25`</t>
+    <t>no time</t>
   </si>
   <si>
-    <t>no time</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>pt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,15 +140,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="19" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,52 +275,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>11.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.87</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.73</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5.75</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.6199999999999992</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.3899999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>9.08</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>4.3499999999999996</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>20.97</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>1.66</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>1.17</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.93</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.68</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.87</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -320,52 +332,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.61</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1.87</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.29</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.61</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.73</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.38</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.41</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>2.13</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>1.54</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>2.82</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>2.98</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
                   <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.72</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,55 +707,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>8.06</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>3.2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>2.72</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>2.48</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>10.65</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
                   <c:v>26.65</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>23.18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.06</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.60199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.99</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.82</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.42</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>13.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -755,55 +764,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>3.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.4900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>3.6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>3.54</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.08</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.4900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>2.98</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>3.01</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>3.51</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
                   <c:v>3.94</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>3.94</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.5299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.88</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.69</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.95</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2.2599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,6 +1032,407 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7438757655293088E-2"/>
+                  <c:y val="-1.1930227471566097E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$19:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$19:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.3743000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4584999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D7A0-4746-AD14-2217CE4FE0D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2031712912"/>
+        <c:axId val="2031717072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2031712912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2031717072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2031717072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2031712912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1106,6 +1513,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1623,6 +2070,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2215,13 +3178,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A0362B9-128B-40FE-8925-F0BD2EEFC34F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2259,9 +3258,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2294,9 +3293,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2329,9 +3345,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2505,19 +3538,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2540,96 +3574,94 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44936</v>
+        <v>43180</v>
       </c>
       <c r="B2" s="2">
-        <v>0.57638888888888895</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2">
-        <v>5.75</v>
+        <v>11.78</v>
       </c>
       <c r="E2">
-        <v>1.87</v>
+        <v>2.91</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44899</v>
+        <v>43906</v>
       </c>
       <c r="B3" s="2">
-        <v>0.38055555555555554</v>
+        <v>0.48472222222222222</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
-        <v>8.6199999999999992</v>
+        <v>0.68</v>
       </c>
       <c r="E3">
-        <v>2.29</v>
+        <v>1.48</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44899</v>
+        <v>43906</v>
       </c>
       <c r="B4" s="2">
-        <v>0.39583333333333331</v>
+        <v>0.45</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
-        <v>8.73</v>
+        <v>7.87</v>
       </c>
       <c r="E4">
-        <v>2.23</v>
+        <v>2.15</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4">
-        <v>44907</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="C5" s="6" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44494</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1.61</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="D5">
+        <v>1.93</v>
+      </c>
+      <c r="E5">
+        <v>2.72</v>
+      </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44907</v>
+        <v>44899</v>
       </c>
       <c r="B6" s="2">
-        <v>0.39583333333333331</v>
+        <v>0.38055555555555554</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>2.4</v>
+        <v>8.6199999999999992</v>
       </c>
       <c r="E6">
-        <v>1.73</v>
+        <v>2.29</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44906</v>
+        <v>44899</v>
       </c>
       <c r="B7" s="2">
         <v>0.39583333333333331</v>
@@ -2638,493 +3670,581 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>4.3899999999999997</v>
+        <v>8.73</v>
       </c>
       <c r="E7">
-        <v>1.38</v>
+        <v>2.23</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44906</v>
       </c>
       <c r="B8" s="2">
-        <v>0.36458333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>4.3899999999999997</v>
       </c>
       <c r="E8">
-        <v>1.41</v>
+        <v>1.38</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45323</v>
+        <v>44906</v>
       </c>
       <c r="B9" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.36458333333333331</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>9.08</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>2.13</v>
+        <v>1.41</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>45328</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.40277777777777773</v>
-      </c>
-      <c r="C10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>44907</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="E10">
-        <v>1.54</v>
-      </c>
+      <c r="D10" s="5">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.61</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45341</v>
+        <v>44907</v>
       </c>
       <c r="B11" s="2">
-        <v>0.36944444444444446</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>20.97</v>
+        <v>2.4</v>
       </c>
       <c r="E11">
-        <v>2.82</v>
+        <v>1.73</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45341</v>
+        <v>44936</v>
       </c>
       <c r="B12" s="2">
-        <v>0.40208333333333335</v>
+        <v>0.57638888888888895</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12">
-        <v>1.66</v>
+        <v>5.75</v>
       </c>
       <c r="E12">
-        <v>2.98</v>
+        <v>1.87</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>45342</v>
+        <v>45323</v>
       </c>
       <c r="B13" s="2">
-        <v>0.38125000000000003</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>1.17</v>
+        <v>9.08</v>
       </c>
       <c r="E13">
-        <v>1.25</v>
+        <v>2.13</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44494</v>
+        <v>45328</v>
       </c>
       <c r="B14" s="2">
-        <v>0.46180555555555558</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>1.93</v>
+        <v>4.3499999999999996</v>
       </c>
       <c r="E14">
-        <v>2.72</v>
+        <v>1.54</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43906</v>
+        <v>45341</v>
       </c>
       <c r="B15" s="2">
-        <v>0.48472222222222222</v>
+        <v>0.36944444444444446</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15">
-        <v>0.68</v>
+        <v>20.97</v>
       </c>
       <c r="E15">
-        <v>1.48</v>
+        <v>2.82</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43906</v>
+        <v>45341</v>
       </c>
       <c r="B16" s="2">
-        <v>0.45</v>
+        <v>0.40208333333333335</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16">
-        <v>7.87</v>
+        <v>1.66</v>
       </c>
       <c r="E16">
-        <v>2.15</v>
+        <v>2.98</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43180</v>
+        <v>45342</v>
       </c>
       <c r="B17" s="2">
-        <v>0.63888888888888895</v>
+        <v>0.38125000000000003</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17">
-        <v>11.78</v>
+        <v>1.17</v>
       </c>
       <c r="E17">
-        <v>2.91</v>
+        <v>1.25</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44899</v>
+        <v>43109</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18">
-        <v>8.06</v>
+        <v>13.7</v>
       </c>
       <c r="E18">
-        <v>3.6</v>
+        <v>3.48</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44899</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
+        <v>43509</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.5</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19">
-        <v>3.2</v>
+        <v>0.9</v>
       </c>
       <c r="E19">
-        <v>3.54</v>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="F19">
+        <v>1.3743000000000001</v>
+      </c>
+      <c r="I19">
+        <f>E19-F19</f>
+        <v>0.88569999999999971</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44873</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
+        <v>43510</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.44444444444444442</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20">
-        <v>3.2</v>
+        <v>1.42</v>
       </c>
       <c r="E20">
-        <v>3.08</v>
+        <v>2.95</v>
+      </c>
+      <c r="F20">
+        <v>2.4584999999999999</v>
+      </c>
+      <c r="H20">
+        <f>77/2.54</f>
+        <v>30.314960629921259</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20:I25" si="0">E20-F20</f>
+        <v>0.49150000000000027</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44873</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
+        <v>43907</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.40277777777777773</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21">
-        <v>0.08</v>
-      </c>
-      <c r="E21">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="G21" t="s">
-        <v>13</v>
+        <v>1.82</v>
+      </c>
+      <c r="E21" s="6">
+        <v>2.69</v>
+      </c>
+      <c r="F21">
+        <v>1.55</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44906</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.35416666666666669</v>
+        <v>44265</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.43402777777777773</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22">
-        <v>2.72</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="E22">
-        <v>2.98</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F22">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>1.2249999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1">
-        <v>44906</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23">
-        <v>2.48</v>
-      </c>
-      <c r="E23">
-        <v>3.01</v>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>45323</v>
+        <v>44544</v>
       </c>
       <c r="B24" s="2">
-        <v>0.3888888888888889</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24">
-        <v>10.65</v>
+        <v>1.06</v>
       </c>
       <c r="E24">
-        <v>3.51</v>
+        <v>3.31</v>
+      </c>
+      <c r="F24">
+        <v>1.81</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>45341</v>
+        <v>44558</v>
       </c>
       <c r="B25" s="2">
-        <v>0.38541666666666669</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25">
-        <v>26.65</v>
+        <v>0.35</v>
       </c>
       <c r="E25">
-        <v>3.94</v>
-      </c>
-      <c r="G25" t="s">
-        <v>16</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F25">
+        <v>0.98</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>0.12000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>45341</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.34791666666666665</v>
+        <v>44873</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26">
-        <v>23.18</v>
+        <v>3.2</v>
       </c>
       <c r="E26">
-        <v>3.94</v>
+        <v>3.08</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44544</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.45833333333333331</v>
+        <v>44873</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
       </c>
       <c r="D27">
-        <v>1.06</v>
+        <v>0.08</v>
       </c>
       <c r="E27">
-        <v>3.31</v>
-      </c>
-      <c r="F27">
-        <v>1.81</v>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27">
+        <f>AVERAGE(I19:I25)</f>
+        <v>0.76602857142857139</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1">
-        <v>44558</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0.11458333333333333</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>44899</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D28">
-        <v>0.35</v>
-      </c>
-      <c r="E28">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F28">
-        <v>0.98</v>
+      <c r="D28" s="8">
+        <v>8.06</v>
+      </c>
+      <c r="E28" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.78600000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="1">
-        <v>44265</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>44899</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D29">
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="E29">
-        <v>2.5299999999999998</v>
+      <c r="D29" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="E29" s="8">
+        <v>3.54</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1">
-        <v>44494</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.4909722222222222</v>
-      </c>
-      <c r="C30" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>44906</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D30">
-        <v>1.99</v>
-      </c>
-      <c r="E30">
-        <v>2.88</v>
+      <c r="D30" s="8">
+        <v>2.72</v>
+      </c>
+      <c r="E30" s="8">
+        <v>2.98</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="G30" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1">
-        <v>43907</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0.40277777777777773</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>44906</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D31">
-        <v>1.82</v>
-      </c>
-      <c r="E31" s="7">
-        <v>2.69</v>
+      <c r="D31" s="8">
+        <v>2.48</v>
+      </c>
+      <c r="E31" s="8">
+        <v>3.01</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43510</v>
+        <v>45323</v>
       </c>
       <c r="B32" s="2">
-        <v>0.44444444444444442</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
       </c>
       <c r="D32">
-        <v>1.42</v>
+        <v>10.65</v>
       </c>
       <c r="E32">
-        <v>2.95</v>
-      </c>
-      <c r="H32">
-        <f>77/2.54</f>
-        <v>30.314960629921259</v>
+        <v>3.51</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43509</v>
+        <v>45341</v>
       </c>
       <c r="B33" s="2">
-        <v>0.5</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="C33" t="s">
         <v>9</v>
       </c>
       <c r="D33">
-        <v>0.9</v>
+        <v>26.65</v>
       </c>
       <c r="E33">
-        <v>2.2599999999999998</v>
+        <v>3.94</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43109</v>
-      </c>
-      <c r="B34" t="s">
-        <v>18</v>
+        <v>45341</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.34791666666666665</v>
       </c>
       <c r="C34" t="s">
         <v>9</v>
       </c>
       <c r="D34">
-        <v>13.7</v>
+        <v>23.18</v>
       </c>
       <c r="E34">
-        <v>3.48</v>
+        <v>3.94</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>44494</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>1.99</v>
+      </c>
+      <c r="E35">
+        <v>2.88</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G34">
-    <sortCondition ref="C2:C34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H34">
+    <sortCondition ref="C1:C34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>